<commit_message>
second version working bot
</commit_message>
<xml_diff>
--- a/DataBase/Courses.xlsx
+++ b/DataBase/Courses.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programing\Prog_Py\PP(poshlo-poehalo)\MEPHI-pp\DataBase\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vladimir\PycharmProjects\MEPHI-pp\DataBase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56777A61-706F-4FF9-B694-B7896825D83B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0473303D-1F70-4894-88B3-0024861EDC51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11746" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="148">
   <si>
     <t>ID</t>
   </si>
@@ -43,166 +43,22 @@
     <t>Skills</t>
   </si>
   <si>
-    <t>Введение в программирование на Go</t>
-  </si>
-  <si>
-    <t>Курс на базовом уровне освещает практические основы программирования на языке Go. Вы научитесь основным конструкциям языка, писать и читать программный код, а также решать алгоритмические задачи. Курс состоит из 6 модулей, каждый из которых включает теорию и практику. 70% времени посвящено практическим заданиям, которые помогут натренировать ваши навыки. Автоматическая система проверки обеспечит быструю обратную связь, а команда курса всегда готова помочь при возникновении вопросов.</t>
-  </si>
-  <si>
-    <t>https://stepik.org/course/158385/promo?search=6104329626</t>
-  </si>
-  <si>
     <t>30-40 часов</t>
   </si>
   <si>
     <t>free</t>
   </si>
   <si>
-    <t>Programming Basics, Go Syntax, Code Reading, Code Analysis, Algorithmic Problem Solving, Data Types, Variables, Conditional Statements, Loops, Functions</t>
-  </si>
-  <si>
-    <t>Полный курс Go: от новичка до профессионала</t>
-  </si>
-  <si>
-    <t>Курс начинается с основ Go, включая объявление переменных, функций и управление типами данных. Затем вы изучите массивы, срезы, мапы и указатели. Дальше мы перейдём к структурам, их методам и валидации данных. Проект будет разбит на пакеты, а также рассмотрена работа с операционной системой. В конце курса вы освоите интерфейсы, внедрение зависимостей, работу с переменными окружения, HTTP-запросами и написание тестов. Практическая часть включает создание пяти проектов, от простого конвертора валют до менеджера паролей.</t>
-  </si>
-  <si>
-    <t>https://stepik.org/course/211704/promo?search=6104329623</t>
-  </si>
-  <si>
     <t>40 часов</t>
   </si>
   <si>
-    <t>2,969 RUB</t>
-  </si>
-  <si>
-    <t>Writing Go code, Decomposing applications into packages, Working with data types, Creating arrays, slices, maps, and structs, Using interfaces and DI, Managing external dependencies, Working with OS and encryption, Making HTTP requests, Writing tests, Working with environment variables</t>
-  </si>
-  <si>
-    <t>Практический Тренажер по Go</t>
-  </si>
-  <si>
-    <t>Этот курс на платформе Stepik представляет собой полный практический тренажер для начинающих программистов на Go. Вы научитесь работать с переменными, типами данных, условными конструкциями, циклами, функциями, массивами и строками. Курс включает задачи для подготовки к собеседованиям, что поможет вам уверенно отвечать на вопросы ведущих технологических компаний. Регулярные обновления и активное сообщество поддерживают ваш интерес и способствуют непрерывному развитию.</t>
-  </si>
-  <si>
-    <t>https://stepik.org/course/175966/promo?search=6104667384</t>
-  </si>
-  <si>
-    <t>899 RUB</t>
-  </si>
-  <si>
-    <t>Variables, Data Types, Control Structures, Functions, Arrays, Strings, Problem Solving, Algorithmic Thinking, Interview Preparation, Logical Thinking</t>
-  </si>
-  <si>
-    <t>Базовые структуры данных и их применение</t>
-  </si>
-  <si>
-    <t>Курс охватывает основные структуры данных, такие как массивы, связные списки, стеки, очереди, множества и хэш-таблицы. Вы научитесь выбирать оптимальные способы их использования, находить преимущества и недостатки каждой структуры, а также успешно применять их на практике. Курс состоит из 6 модулей, каждый из которых включает теорию, собственные и готовые реализации, а также практические задания. Автоматическая система проверки обеспечивает быструю обратную связь, а команда курса всегда готова помочь при возникновении вопросов.</t>
-  </si>
-  <si>
-    <t>https://stepik.org/course/187922/promo?search=6104667386</t>
-  </si>
-  <si>
-    <t>30 часов</t>
-  </si>
-  <si>
-    <t>4,193 RUB</t>
-  </si>
-  <si>
-    <t>Data Structures, Optimization Techniques, Algorithmic Thinking, Problem Solving, Code Optimization, Interview Preparation, Practical Implementation, Theoretical Understanding, Data Analysis, Big Data Processing</t>
-  </si>
-  <si>
-    <t>Профессиональная разработка на Go (Golang)</t>
-  </si>
-  <si>
-    <t>Этот курс предназначен для опытных разработчиков и студентов старших курсов ИТ-специальностей, желающих освоить язык Go (Golang). Вы научитесь создавать высококонкурентные приложения, работать с веб-разработкой на серверной стороне, оптимизировать код и использовать инструменты отладки и тестирования. Предварительные требования включают крепкие практические навыки программирования, знание основ работы веба и работы в командной строке Linux, а также понимание протокола HTTP. Курс не подходит для начинающих программистов.</t>
-  </si>
-  <si>
-    <t>https://stepik.org/course/187490/promo?search=6104667388</t>
-  </si>
-  <si>
-    <t>Go Programming, Concurrency, Web Development, Server-Side Development, Linux Command Line, HTTP Protocol, Code Optimization, Debugging, Testing, Performance Tuning</t>
-  </si>
-  <si>
-    <t>Искусство работы с ошибками в Go</t>
-  </si>
-  <si>
-    <t>Этот курс представляет первую часть специализации "Искусство работы с ошибками и безмолвной паники в Go". Вы узнаете о различных способах обработки ошибок, их подводных камнях и лучших практиках. Курс охватывает работу с ошибками в конкурентном коде, логирование, использование стандартной библиотеки и сторонних модулей. Вы будете читать исходный код, решать задачи и проходить тесты, чтобы сделать ваш код production ready. Курс предназначен как для новичков, так и для опытных Go-разработчиков.</t>
-  </si>
-  <si>
-    <t>https://stepik.org/course/89381/promo?search=6104695260</t>
-  </si>
-  <si>
-    <t>20-25 часов</t>
-  </si>
-  <si>
-    <t>18,600 RUB</t>
-  </si>
-  <si>
-    <t>Error Handling, Go Standard Library, Concurrency, Testing, Stack Traces, Constant Errors, Error Methods, Logging, External Modules Compatibility, Best Practices</t>
-  </si>
-  <si>
-    <t>Разработка бэкенда на Go: от идеи до продукта</t>
-  </si>
-  <si>
-    <t>Курс направлен на разработку бэкенда для чата поддержки банка с использованием языка Go. Вы научитесь реализовывать функциональные и нефункциональные требования, проектировать и разрабатывать API, работать с инструментарием Go, читать и писать тесты, а также обеспечивать безопасность и масштабируемость приложения. Курс состоит из 7 основных модулей и 2 дополнительных, посвященных горизонтальному масштабированию и деплою.</t>
-  </si>
-  <si>
-    <t>https://stepik.org/course/105653/promo?search=6104695262</t>
-  </si>
-  <si>
     <t>80 часов</t>
   </si>
   <si>
-    <t>62,000 RUB</t>
-  </si>
-  <si>
-    <t>Functional Requirements, Non-Functional Requirements, Go Service Development, API Design, Go Tooling, Code Reading, Test Writing, Security, Scalability, Deployment</t>
-  </si>
-  <si>
-    <t>Разработка Микросервисов на Go с gRPC и Облачными Технологиями</t>
-  </si>
-  <si>
-    <t>Этот курс, проводимый Senior Engineer из BigTech, фокусируется на разработке высокопроизводительных и масштабируемых микросервисов на языке Go. Вы научитесь создавать gRPC-серверы, развертывать сервисы в облаке, работать с базами данных PostgreSQL и Redis, а также применять лучшие практики и нюансы построения микросервисов, используемые в крупных компаниях.</t>
-  </si>
-  <si>
-    <t>https://olezhek28.courses/</t>
-  </si>
-  <si>
-    <t>45 000 RUB</t>
-  </si>
-  <si>
-    <t>Microservices Architecture, Go Programming, gRPC, Cloud Deployment, PostgreSQL, Redis, Scalability, Performance Optimization, Best Practices, DevOps</t>
-  </si>
-  <si>
-    <t>Разработка микросервисов на Go</t>
-  </si>
-  <si>
-    <t>Курс предназначен для начинающих и опытных Go-разработчиков, желающих освоить разработку микросервисов. Вы научитесь работать с базами данных PostgreSQL и MongoDB, использовать Apache Kafka для обмена данными, создавать шаблоны сервисов по принципам гексагональной архитектуры и обеспечивать наблюдаемость микросервисных приложений.</t>
-  </si>
-  <si>
-    <t>https://www.hse.ru/edu/courses/646508391</t>
-  </si>
-  <si>
-    <t>Go, PostgreSQL, MongoDB, Apache Kafka, Hexagonal Architecture, Observability, Service Template Development, Microservices, Database Integration, Middleware Communication</t>
-  </si>
-  <si>
-    <t>Разработка микросервисов REST на Golang</t>
-  </si>
-  <si>
-    <t>Этот курс охватывает все этапы разработки микросервисов на Golang, начиная с проектирования и заканчивая производственными метриками. Вы научитесь работать с базами данных MySQL, Cassandra и Elasticsearch, а также применять шаблоны проектирования, такие как MVC и Domain Driven Design. Курс поможет вам создавать эффективные и масштабируемые микросервисы.</t>
-  </si>
-  <si>
-    <t>https://coursehunter.net/course/golang-polnoe-rukovodstvo-po-mikroservisam-v-go-chast-1</t>
-  </si>
-  <si>
     <t>20 часов</t>
   </si>
   <si>
     <t>1000 RUB</t>
-  </si>
-  <si>
-    <t>Go, RESTful API Design, Microservices Architecture, MySQL, Cassandra, Elasticsearch, MVC Pattern, Domain Driven Design, Performance Metrics, Service Deployment</t>
   </si>
   <si>
     <t>Программирование на Java и основы веб-разработки</t>
@@ -982,10 +838,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" workbookViewId="0">
-      <selection activeCell="M38" sqref="M38"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="55" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1024,137 +880,137 @@
     </row>
     <row r="2" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="3">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="3">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="3">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="3">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="3">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="3">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>39</v>
@@ -1162,7 +1018,7 @@
     </row>
     <row r="8" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="3">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>40</v>
@@ -1174,56 +1030,56 @@
         <v>42</v>
       </c>
       <c r="E8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="G8" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="3">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="3" t="s">
+      <c r="G9" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="3">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>53</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>11</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>54</v>
@@ -1231,7 +1087,7 @@
     </row>
     <row r="11" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="3">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>55</v>
@@ -1254,7 +1110,7 @@
     </row>
     <row r="12" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="3">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>61</v>
@@ -1269,7 +1125,7 @@
         <v>64</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>65</v>
@@ -1277,7 +1133,7 @@
     </row>
     <row r="13" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="3">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>66</v>
@@ -1289,33 +1145,33 @@
         <v>68</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="3">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>73</v>
+        <v>8</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>74</v>
@@ -1323,7 +1179,7 @@
     </row>
     <row r="15" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="3">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>75</v>
@@ -1335,10 +1191,10 @@
         <v>77</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>78</v>
@@ -1346,7 +1202,7 @@
     </row>
     <row r="16" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="3">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>79</v>
@@ -1358,10 +1214,10 @@
         <v>81</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>82</v>
+        <v>8</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>83</v>
@@ -1369,7 +1225,7 @@
     </row>
     <row r="17" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="3">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>84</v>
@@ -1381,10 +1237,10 @@
         <v>86</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>87</v>
@@ -1392,7 +1248,7 @@
     </row>
     <row r="18" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="3">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>88</v>
@@ -1404,542 +1260,312 @@
         <v>90</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>43</v>
+        <v>9</v>
       </c>
       <c r="F18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G18" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="3">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="E19" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="3">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="E20" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="3">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G21" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="3">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>112</v>
+        <v>16</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>11</v>
+        <v>107</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="3">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>117</v>
+        <v>9</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>11</v>
+        <v>112</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="3">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>58</v>
+        <v>16</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>11</v>
+        <v>117</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="3">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>117</v>
+        <v>9</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>126</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="3">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>130</v>
+        <v>9</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="3">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>117</v>
+        <v>11</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="3">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>16</v>
+        <v>133</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="3">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>117</v>
+        <v>69</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="3">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="3">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>64</v>
+        <v>11</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>11</v>
+        <v>146</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="3">
-        <v>31</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A33" s="3">
-        <v>32</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="3">
-        <v>33</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="3">
-        <v>34</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="3">
-        <v>35</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="3">
-        <v>36</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="F37" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="3">
-        <v>37</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="3">
-        <v>38</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="F39" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="3">
-        <v>39</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F40" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A41" s="3">
-        <v>40</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="F41" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>195</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>

</xml_diff>